<commit_message>
solved bug of dataset creation for v2: edge case if same theme present in different source and finished translation
</commit_message>
<xml_diff>
--- a/book_themes_alignment_data/Juliette_assignments_v1_v2.xlsx
+++ b/book_themes_alignment_data/Juliette_assignments_v1_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dre\Documents\projet biblio scolaire\Books-Python\book_themes_alignment_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B301EA8-4FB5-4E4E-B513-9F51FA678DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0259DF67-5069-4CD2-8A25-6654BAF09128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="21600" windowHeight="11295" xr2:uid="{5006917A-C890-44C3-9BCB-649A38B05E11}"/>
+    <workbookView xWindow="1560" yWindow="1575" windowWidth="21600" windowHeight="11295" xr2:uid="{5006917A-C890-44C3-9BCB-649A38B05E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="212">
   <si>
     <t>UUID</t>
   </si>
@@ -663,13 +663,22 @@
   </si>
   <si>
     <t>WBJ</t>
+  </si>
+  <si>
+    <t>4de94b55e-538e-4225-93f3-303390e81ed8</t>
+  </si>
+  <si>
+    <t>champignon</t>
+  </si>
+  <si>
+    <t>PSQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,6 +690,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -718,11 +734,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1057,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF3FD6E-2F0B-4BDB-93A8-729F353D25D7}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:D69"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,6 +1877,17 @@
         <v>208</v>
       </c>
     </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B70" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>